<commit_message>
fixed 2 column vs 3 column confusion
</commit_message>
<xml_diff>
--- a/docs/Data/IllinoisBirthWeights.xlsx
+++ b/docs/Data/IllinoisBirthWeights.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Desktop\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD8653D4-4BB7-429D-B329-73590671E56C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDEA4982-B87C-46B9-AA2D-F605B60BD404}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="2600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+  <si>
+    <t>Black_US</t>
+  </si>
+  <si>
+    <t>Black_Africa</t>
+  </si>
+  <si>
+    <t>White_US</t>
+  </si>
   <si>
     <t>Comments</t>
   </si>
@@ -59,22 +68,19 @@
     <t>The data are representive of birthweights (in grams)</t>
   </si>
   <si>
-    <t>Born in US</t>
-  </si>
-  <si>
-    <t>Born in Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">of children born in Illinois to mothers are of </t>
-  </si>
-  <si>
-    <t xml:space="preserve">African descent. The columns indicate whether </t>
-  </si>
-  <si>
-    <t>the mother was born in the United States or</t>
-  </si>
-  <si>
-    <t>in Africa.</t>
+    <t>of children born in Illinois to mothers who fall into</t>
+  </si>
+  <si>
+    <t>one of the following categories:</t>
+  </si>
+  <si>
+    <t>(1) Black, born in the United States (Black_US)</t>
+  </si>
+  <si>
+    <t>(2) Black, born in Africa (Black_Africa), or</t>
+  </si>
+  <si>
+    <t>(3) White, born in the United States (White_US).</t>
   </si>
 </sst>
 </file>
@@ -450,359 +456,598 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2566</v>
       </c>
       <c r="B2">
         <v>2790</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>4429</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3068</v>
       </c>
       <c r="B3">
         <v>3283</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>3191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2931</v>
       </c>
       <c r="B4">
         <v>3148</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>3712</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2882</v>
       </c>
       <c r="B5">
         <v>3101</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>3399</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2022</v>
       </c>
       <c r="B6">
         <v>2257</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>2638</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2073</v>
       </c>
       <c r="B7">
         <v>2307</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>3946</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2907</v>
       </c>
       <c r="B8">
         <v>3125</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>3173</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4028</v>
       </c>
       <c r="B9">
         <v>4225</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>2926</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2982</v>
       </c>
       <c r="B10">
         <v>3199</v>
       </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>2303</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2907</v>
       </c>
       <c r="B11">
         <v>3125</v>
       </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>3885</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2893</v>
       </c>
       <c r="B12">
         <v>3112</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>3208</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2422</v>
       </c>
       <c r="B13">
         <v>2649</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>2969</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3910</v>
       </c>
       <c r="B14">
         <v>4109</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>2948</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2588</v>
       </c>
       <c r="B15">
         <v>2812</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>2270</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2832</v>
       </c>
       <c r="B16">
         <v>3051</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>3172</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2063</v>
       </c>
       <c r="B17">
         <v>2297</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>2318</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2213</v>
       </c>
       <c r="B18">
         <v>2444</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>2456</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3672</v>
       </c>
       <c r="B19">
         <v>3875</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>3661</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3512</v>
       </c>
       <c r="B20">
         <v>3718</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>3854</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3425</v>
       </c>
       <c r="B21">
         <v>3633</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>3122</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3097</v>
       </c>
       <c r="B22">
         <v>3312</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>3666</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2583</v>
       </c>
       <c r="B23">
         <v>2807</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>4414</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3961</v>
       </c>
       <c r="B24">
         <v>4159</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>3490</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2936</v>
       </c>
       <c r="B25">
         <v>3154</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>3871</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>3081</v>
       </c>
       <c r="B26">
         <v>3296</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>2679</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>3873</v>
       </c>
       <c r="B27">
         <v>4073</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <v>2850</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2966</v>
       </c>
       <c r="B28">
         <v>3183</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>2852</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2906</v>
       </c>
       <c r="B29">
         <v>3124</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>3316</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3489</v>
       </c>
       <c r="B30">
         <v>3696</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>3596</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2525</v>
       </c>
       <c r="B31">
         <v>2751</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>2719</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3087</v>
       </c>
       <c r="B32">
         <v>3302</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>4448</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3697</v>
       </c>
       <c r="B33">
         <v>3900</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>3043</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2293</v>
       </c>
       <c r="B34">
         <v>2523</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>2709</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2928</v>
       </c>
       <c r="B35">
         <v>3146</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>3695</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2641</v>
       </c>
       <c r="B36">
         <v>2864</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>3583</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>3126</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>2867</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>2661</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>4056</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>3951</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>3342</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>4068</v>
+      </c>
+      <c r="C40">
+        <v>3124</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>4281</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C42">
+        <v>3839</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <v>3458</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>3931</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C45">
+        <v>4322</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix 2 column vs. 3 column file confusion
</commit_message>
<xml_diff>
--- a/docs/Data/IllinoisBirthWeights.xlsx
+++ b/docs/Data/IllinoisBirthWeights.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Desktop\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD8653D4-4BB7-429D-B329-73590671E56C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDEA4982-B87C-46B9-AA2D-F605B60BD404}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="2600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+  <si>
+    <t>Black_US</t>
+  </si>
+  <si>
+    <t>Black_Africa</t>
+  </si>
+  <si>
+    <t>White_US</t>
+  </si>
   <si>
     <t>Comments</t>
   </si>
@@ -59,22 +68,19 @@
     <t>The data are representive of birthweights (in grams)</t>
   </si>
   <si>
-    <t>Born in US</t>
-  </si>
-  <si>
-    <t>Born in Africa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">of children born in Illinois to mothers are of </t>
-  </si>
-  <si>
-    <t xml:space="preserve">African descent. The columns indicate whether </t>
-  </si>
-  <si>
-    <t>the mother was born in the United States or</t>
-  </si>
-  <si>
-    <t>in Africa.</t>
+    <t>of children born in Illinois to mothers who fall into</t>
+  </si>
+  <si>
+    <t>one of the following categories:</t>
+  </si>
+  <si>
+    <t>(1) Black, born in the United States (Black_US)</t>
+  </si>
+  <si>
+    <t>(2) Black, born in Africa (Black_Africa), or</t>
+  </si>
+  <si>
+    <t>(3) White, born in the United States (White_US).</t>
   </si>
 </sst>
 </file>
@@ -450,359 +456,598 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2566</v>
       </c>
       <c r="B2">
         <v>2790</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>4429</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3068</v>
       </c>
       <c r="B3">
         <v>3283</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>3191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2931</v>
       </c>
       <c r="B4">
         <v>3148</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>3712</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2882</v>
       </c>
       <c r="B5">
         <v>3101</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>3399</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2022</v>
       </c>
       <c r="B6">
         <v>2257</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>2638</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2073</v>
       </c>
       <c r="B7">
         <v>2307</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>3946</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2907</v>
       </c>
       <c r="B8">
         <v>3125</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>3173</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4028</v>
       </c>
       <c r="B9">
         <v>4225</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>2926</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2982</v>
       </c>
       <c r="B10">
         <v>3199</v>
       </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>2303</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2907</v>
       </c>
       <c r="B11">
         <v>3125</v>
       </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>3885</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2893</v>
       </c>
       <c r="B12">
         <v>3112</v>
       </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>3208</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2422</v>
       </c>
       <c r="B13">
         <v>2649</v>
       </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>2969</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3910</v>
       </c>
       <c r="B14">
         <v>4109</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>2948</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2588</v>
       </c>
       <c r="B15">
         <v>2812</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>2270</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2832</v>
       </c>
       <c r="B16">
         <v>3051</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>3172</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2063</v>
       </c>
       <c r="B17">
         <v>2297</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>2318</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2213</v>
       </c>
       <c r="B18">
         <v>2444</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>2456</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3672</v>
       </c>
       <c r="B19">
         <v>3875</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>3661</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3512</v>
       </c>
       <c r="B20">
         <v>3718</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>3854</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3425</v>
       </c>
       <c r="B21">
         <v>3633</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>3122</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3097</v>
       </c>
       <c r="B22">
         <v>3312</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>3666</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2583</v>
       </c>
       <c r="B23">
         <v>2807</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>4414</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3961</v>
       </c>
       <c r="B24">
         <v>4159</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>3490</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2936</v>
       </c>
       <c r="B25">
         <v>3154</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>3871</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>3081</v>
       </c>
       <c r="B26">
         <v>3296</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>2679</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>3873</v>
       </c>
       <c r="B27">
         <v>4073</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <v>2850</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2966</v>
       </c>
       <c r="B28">
         <v>3183</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>2852</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2906</v>
       </c>
       <c r="B29">
         <v>3124</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>3316</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3489</v>
       </c>
       <c r="B30">
         <v>3696</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>3596</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2525</v>
       </c>
       <c r="B31">
         <v>2751</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>2719</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>3087</v>
       </c>
       <c r="B32">
         <v>3302</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>4448</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>3697</v>
       </c>
       <c r="B33">
         <v>3900</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>3043</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2293</v>
       </c>
       <c r="B34">
         <v>2523</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>2709</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2928</v>
       </c>
       <c r="B35">
         <v>3146</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>3695</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2641</v>
       </c>
       <c r="B36">
         <v>2864</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>3583</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>3126</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>2867</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>2661</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>4056</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>3951</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>3342</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>4068</v>
+      </c>
+      <c r="C40">
+        <v>3124</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>4281</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C42">
+        <v>3839</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <v>3458</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>3931</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C45">
+        <v>4322</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>